<commit_message>
output with fixed portfolios
</commit_message>
<xml_diff>
--- a/output/Portfolio Robustness 2024-02-29_2.xlsx
+++ b/output/Portfolio Robustness 2024-02-29_2.xlsx
@@ -497,37 +497,37 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>-0.9629055821482745</v>
+        <v>-0.9876306439548168</v>
       </c>
       <c r="F2">
-        <v>0.428</v>
+        <v>0.1419999999999999</v>
       </c>
       <c r="G2">
-        <v>0.06506839249674191</v>
+        <v>0.05329184960510227</v>
       </c>
       <c r="H2">
-        <v>0.142</v>
+        <v>-0.2870000000000001</v>
       </c>
       <c r="I2">
-        <v>0.6973825581271207</v>
+        <v>0.6935707421018915</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>0.2499999999999999</v>
       </c>
       <c r="K2">
-        <v>0.02457325187167923</v>
+        <v>0.01228662593583961</v>
       </c>
       <c r="L2">
-        <v>0.5</v>
+        <v>0.2499999999999999</v>
       </c>
       <c r="M2">
-        <v>-18.84732735459614</v>
+        <v>-19.09732735459614</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
+        <v>0.2499999999999999</v>
       </c>
       <c r="O2">
-        <v>0.3782050955033748</v>
+        <v>0.3703728708744926</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -535,31 +535,31 @@
         </is>
       </c>
       <c r="Q2">
-        <v>0.3580949162788734</v>
+        <v>0.3500093807272507</v>
       </c>
       <c r="R2">
-        <v>0.142</v>
+        <v>-0.2870000000000001</v>
       </c>
       <c r="S2">
-        <v>-0.02186693097755732</v>
+        <v>-0.03473852462743127</v>
       </c>
       <c r="T2">
-        <v>-0.716</v>
+        <v>-1.574</v>
       </c>
       <c r="U2">
-        <v>-1.043733861955115</v>
+        <v>-1.069477049254862</v>
       </c>
       <c r="V2">
-        <v>0.4279999999999999</v>
+        <v>0.1419999999999997</v>
       </c>
       <c r="W2">
-        <v>0.3187553793482952</v>
+        <v>0.3101743169150459</v>
       </c>
       <c r="X2">
-        <v>0.142</v>
+        <v>-0.2870000000000001</v>
       </c>
       <c r="Y2">
-        <v>-0.2131216352451893</v>
+        <v>-0.2284023026818084</v>
       </c>
     </row>
     <row r="3">
@@ -575,40 +575,40 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-1.217340228967041</v>
+        <v>-1.615833352300119</v>
       </c>
       <c r="F3">
-        <v>0.5043334404089502</v>
+        <v>0.4152538698122384</v>
       </c>
       <c r="G3">
-        <v>-18.78</v>
+        <v>-28.67000000000001</v>
       </c>
       <c r="H3">
-        <v>0.03630982356432427</v>
+        <v>-0.1368814184996674</v>
       </c>
       <c r="I3">
-        <v>-18.78</v>
+        <v>-28.67000000000001</v>
       </c>
       <c r="J3">
-        <v>0.2643994448208332</v>
+        <v>0.1321997224104166</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L3">
-        <v>-0.349859615665607</v>
+        <v>-0.5924519644989494</v>
       </c>
       <c r="M3">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N3">
-        <v>0.8254693865386175</v>
+        <v>0.794103316340241</v>
       </c>
       <c r="O3">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P3">
-        <v>0.7995524433013794</v>
+        <v>0.7635286649520693</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -616,28 +616,28 @@
         </is>
       </c>
       <c r="R3">
-        <v>-0.08702579554566449</v>
+        <v>-0.2823825111059153</v>
       </c>
       <c r="S3">
-        <v>0.05809523809523798</v>
+        <v>-0.4128571428571431</v>
       </c>
       <c r="T3">
-        <v>-1.174051591091329</v>
+        <v>-1.564765022211831</v>
       </c>
       <c r="U3">
-        <v>-0.883809523809524</v>
+        <v>-1.825714285714286</v>
       </c>
       <c r="V3">
-        <v>0.2753161363028903</v>
+        <v>0.1450783259293897</v>
       </c>
       <c r="W3">
-        <v>0.3720634920634919</v>
+        <v>0.05809523809523783</v>
       </c>
       <c r="X3">
-        <v>-1.045383231618577</v>
+        <v>-1.412972806611539</v>
       </c>
       <c r="Y3">
-        <v>0.03512195121951221</v>
+        <v>-0.4473170731707318</v>
       </c>
     </row>
     <row r="4">
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.4905511456615432</v>
+        <v>0.4968884168487733</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.5490092197236439</v>
+        <v>0.6177126501117919</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -733,10 +733,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>-0.7482517482517482</v>
+        <v>-0.1655011655011654</v>
       </c>
       <c r="C6">
-        <v>-0.06959695444515727</v>
+        <v>-0.05629174057799417</v>
       </c>
       <c r="E6">
         <v>-1.099517832529193</v>
@@ -811,10 +811,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>-1.017485304687593</v>
+        <v>-0.7101438528184884</v>
       </c>
       <c r="C7">
-        <v>0.949443882709808</v>
+        <v>0.9662959218065386</v>
       </c>
       <c r="D7">
         <v>-3.473451327433628</v>
@@ -889,10 +889,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>-0.1655011655011655</v>
+        <v>0.2229992229992231</v>
       </c>
       <c r="C8">
-        <v>-2.304502191978976</v>
+        <v>-2.263395952655775</v>
       </c>
       <c r="E8">
         <v>-5.48642579885674</v>
@@ -967,10 +967,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>-0.03767790152081919</v>
+        <v>0.1204007878678399</v>
       </c>
       <c r="C9">
-        <v>0.949443882709808</v>
+        <v>0.9662959218065386</v>
       </c>
       <c r="D9">
         <v>-1.300884955752212</v>
@@ -1045,10 +1045,10 @@
         </is>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <v>-0.3333333333333332</v>
       </c>
       <c r="C10">
-        <v>-0.02519230882158107</v>
+        <v>-0.01243946498900145</v>
       </c>
       <c r="E10">
         <v>-1.012355705761359</v>
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.3594334492534941</v>
+        <v>-0.1523388800676773</v>
       </c>
       <c r="C11">
-        <v>-1</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="D11">
         <v>-2.014326475633197</v>
@@ -1201,10 +1201,10 @@
         </is>
       </c>
       <c r="B12">
-        <v>-1</v>
+        <v>-0.3333333333333332</v>
       </c>
       <c r="C12">
-        <v>0.9496153823568378</v>
+        <v>0.9502421400439942</v>
       </c>
       <c r="E12">
         <v>0.9010997527738305</v>
@@ -1279,10 +1279,10 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.2591822228069943</v>
+        <v>0.3720375733188028</v>
       </c>
       <c r="C13">
-        <v>-1</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="D13">
         <v>-0.642645059703994</v>
@@ -1357,10 +1357,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>-1</v>
+        <v>-0.3333333333333332</v>
       </c>
       <c r="C14">
-        <v>-0.6082473380986473</v>
+        <v>-0.5882416016427144</v>
       </c>
       <c r="E14">
         <v>-2.156837677428938</v>
@@ -1435,10 +1435,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>-4.729653842196944</v>
+        <v>-3.856804792701198</v>
       </c>
       <c r="C15">
-        <v>-1</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="D15">
         <v>-11.70459196235886</v>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>-0.5578627204554848</v>
+        <v>-0.5384837416867083</v>
       </c>
       <c r="E16">
         <v>-2.057937430202768</v>
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>-3.988836065003939</v>
+        <v>-3.228842366020001</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1659,10 +1659,10 @@
         </is>
       </c>
       <c r="B18">
-        <v>-0.1655011655011655</v>
+        <v>0.2229992229992231</v>
       </c>
       <c r="C18">
-        <v>0.02139900051040752</v>
+        <v>0.03357227338176014</v>
       </c>
       <c r="E18">
         <v>-0.9209013645940017</v>
@@ -1737,10 +1737,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.08005862961327366</v>
+        <v>0.2202014677059118</v>
       </c>
       <c r="C19">
-        <v>-0.06167846309403426</v>
+        <v>0.2922143579373105</v>
       </c>
       <c r="D19">
         <v>-1.039823008849557</v>
@@ -1815,10 +1815,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.4172494172494173</v>
+        <v>0.6114996114996115</v>
       </c>
       <c r="C20">
-        <v>0.5106995002552037</v>
+        <v>0.51678613669088</v>
       </c>
       <c r="E20">
         <v>0.03954931770299911</v>
@@ -1893,10 +1893,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.5400293148066369</v>
+        <v>0.6101007338529558</v>
       </c>
       <c r="C21">
-        <v>0.4691607684529829</v>
+        <v>0.6461071789686553</v>
       </c>
       <c r="D21">
         <v>-0.01991150442477876</v>
@@ -1971,10 +1971,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>-0.7482517482517479</v>
+        <v>-0.1655011655011651</v>
       </c>
       <c r="C22">
-        <v>-0.4679014992343889</v>
+        <v>-0.44964158992736</v>
       </c>
       <c r="E22">
         <v>-1.881352046891003</v>
@@ -2049,10 +2049,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>-0.3799120555800894</v>
+        <v>-0.1696977984411322</v>
       </c>
       <c r="C23">
-        <v>-0.5925176946410512</v>
+        <v>-0.06167846309403407</v>
       </c>
       <c r="D23">
         <v>-2.059734513274336</v>
@@ -2127,10 +2127,10 @@
         </is>
       </c>
       <c r="B24">
-        <v>-0.1655011655011655</v>
+        <v>0.2229992229992231</v>
       </c>
       <c r="C24">
-        <v>0.1756803514613061</v>
+        <v>0.1859344468690492</v>
       </c>
       <c r="E24">
         <v>-0.6180616395911059</v>
@@ -2205,10 +2205,10 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.511094065629614</v>
+        <v>0.5855734481300399</v>
       </c>
       <c r="C25">
-        <v>-0.03640040444893834</v>
+        <v>0.3090663970340412</v>
       </c>
       <c r="D25">
         <v>-0.084070796460177</v>

</xml_diff>